<commit_message>
create wishList page and assertios and Logs
</commit_message>
<xml_diff>
--- a/testdata/testdataexcel.xlsx
+++ b/testdata/testdataexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B88CC0B-23F5-484F-9FBB-3C0B8205F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B74DFA-5AE9-4B94-8986-F27839B74831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="16875" windowHeight="10432" xr2:uid="{AF5F0721-3653-4AF0-80E1-0B0E1838BAF9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AF5F0721-3653-4AF0-80E1-0B0E1838BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
updating logmessage and adding html reports and capturing screenshots for failures
</commit_message>
<xml_diff>
--- a/testdata/testdataexcel.xlsx
+++ b/testdata/testdataexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B74DFA-5AE9-4B94-8986-F27839B74831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96972BE3-E5E3-4D9F-A3C4-ADEAD1C9BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AF5F0721-3653-4AF0-80E1-0B0E1838BAF9}"/>
   </bookViews>
@@ -66,13 +66,13 @@
     <t>Account Login</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>False</t>
   </si>
   <si>
     <t>True</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -475,7 +475,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -489,7 +489,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -517,21 +517,21 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rewrite login test case to enhance reliability and cover dynamic title and error handling
</commit_message>
<xml_diff>
--- a/testdata/testdataexcel.xlsx
+++ b/testdata/testdataexcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96972BE3-E5E3-4D9F-A3C4-ADEAD1C9BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CB1672-7CFF-4C09-878F-04BD6C1A2766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{AF5F0721-3653-4AF0-80E1-0B0E1838BAF9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF5F0721-3653-4AF0-80E1-0B0E1838BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -42,9 +45,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Tittle</t>
-  </si>
-  <si>
     <t>Error Message</t>
   </si>
   <si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>Expected_tittle</t>
   </si>
 </sst>
 </file>
@@ -440,13 +443,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="3" width="12.796875" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" customWidth="1"/>
     <col min="4" max="4" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -458,80 +462,80 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test forgotten password link
</commit_message>
<xml_diff>
--- a/testdata/testdataexcel.xlsx
+++ b/testdata/testdataexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python-Selenium\QA-Automation-Learning\MySecondProject_Opencart\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3603828-1903-4DE2-A5AD-734F56C83DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54E2874-0353-4916-A980-09D356CC14F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF5F0721-3653-4AF0-80E1-0B0E1838BAF9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Account Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>False</t>
@@ -443,7 +440,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -462,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -479,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -493,7 +490,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -507,7 +504,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -521,21 +518,15 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>